<commit_message>
(ABM-812) Correct transit validation template error
</commit_message>
<xml_diff>
--- a/validation/transit_assignment_validation.xlsx
+++ b/validation/transit_assignment_validation.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kulshresthaa\Desktop\Validation Task\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20130" windowHeight="7575" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="boardingByModeRawInput" sheetId="30" r:id="rId1"/>
@@ -17,7 +12,8 @@
     <sheet name="boardingByRouteRawInput" sheetId="31" r:id="rId3"/>
     <sheet name="boardingsByRoute" sheetId="32" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
+  <oleSize ref="A1:R22"/>
 </workbook>
 </file>
 
@@ -56,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="30">
   <si>
     <t>Total</t>
   </si>
@@ -130,9 +126,6 @@
     <t>vol</t>
   </si>
   <si>
-    <t>Scenario 540</t>
-  </si>
-  <si>
     <t>Kiss and Ride to Transit</t>
   </si>
   <si>
@@ -154,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -958,6 +951,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -993,6 +1003,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1171,7 +1198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -1184,13 +1211,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,7 +1225,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5">
         <v>773</v>
@@ -1209,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5">
         <v>2194</v>
@@ -1231,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5">
         <v>687</v>
@@ -1242,7 +1269,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5">
         <v>1691.9999989999999</v>
@@ -1264,7 +1291,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5">
         <v>8494.9999989999997</v>
@@ -1275,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5">
         <v>14367</v>
@@ -1297,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5">
         <v>57</v>
@@ -1308,7 +1335,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5">
         <v>268.999999</v>
@@ -1330,7 +1357,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5">
         <v>5493.0000090000003</v>
@@ -1341,7 +1368,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5">
         <v>4414.9999879999996</v>
@@ -1367,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,10 +2021,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3081,8 +3108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E271"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,15 +3124,13 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="55"/>
       <c r="B1" s="60"/>
-      <c r="C1" s="88" t="s">
-        <v>24</v>
-      </c>
+      <c r="C1" s="88"/>
       <c r="D1" s="89"/>
       <c r="E1" s="90"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="61" t="s">
         <v>12</v>

</xml_diff>